<commit_message>
.m extension to CFX functions ,  function for participant selection was added
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Avances en los TODOs
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="9.5546875" customWidth="true"/>
+    <col min="2" max="2" width="9.5546875" customWidth="true"/>
+    <col min="3" max="3" width="9.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
TODOs to interop case and some function renaming
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Canvis forcasting and service
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="9.5546875" customWidth="true"/>
+    <col min="2" max="2" width="9.5546875" customWidth="true"/>
+    <col min="3" max="3" width="9.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Canvis forecasting and service
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -54,7 +54,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -122,530 +122,530 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>3489</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>2788</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>4529.7630000000008</v>
+        <v>3586</v>
       </c>
       <c r="B11" s="0">
-        <v>2226.753999999999</v>
+        <v>2166</v>
       </c>
       <c r="C11" s="0">
-        <v>2279.1679999999992</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>2365.848</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>4330.2969999999987</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B17" s="0">
-        <v>2277.2980000000002</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C17" s="0">
-        <v>2393.0169999999994</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>2889.52</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>1919.04</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>4436.0550000000012</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B23" s="0">
-        <v>1788.8079999999998</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C23" s="0">
-        <v>1895.6379999999997</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B24" s="0">
-        <v>0</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C24" s="0">
-        <v>0</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>10803.777</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>3701.6649999999995</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B29" s="0">
-        <v>1943.5560000000007</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C29" s="0">
-        <v>1983.7219999999991</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B30" s="0">
-        <v>0</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>1969.172</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>4795.8240000000023</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B35" s="0">
-        <v>2852.4750000000004</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C35" s="0">
-        <v>2852.4190000000003</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5.8399999999996908</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B36" s="0">
-        <v>133.69000000000005</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C36" s="0">
-        <v>121.76000000000067</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>8294.1510000000035</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B41" s="0">
-        <v>4466.217999999998</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C41" s="0">
-        <v>4292.9000000000015</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B42" s="0">
-        <v>0</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>7589.8439999999946</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B47" s="0">
-        <v>4775.7479999999987</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C47" s="0">
-        <v>4709.6369999999997</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B48" s="0">
-        <v>0</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>0</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>0</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>0</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>5089.1450000000059</v>
+        <v>0</v>
       </c>
       <c r="B53" s="0">
-        <v>2495.0159999999996</v>
+        <v>0</v>
       </c>
       <c r="C53" s="0">
-        <v>2607.3530000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -661,57 +661,57 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>0</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>0</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>0</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>0</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>0</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>0</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>0</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>0</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>3628.4829999999993</v>
+        <v>0</v>
       </c>
       <c r="B59" s="0">
-        <v>1841.2869999999996</v>
+        <v>0</v>
       </c>
       <c r="C59" s="0">
-        <v>1956.3139999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -722,138 +722,6 @@
         <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="0">
-        <v>0</v>
-      </c>
-      <c r="B61" s="0">
-        <v>0</v>
-      </c>
-      <c r="C61" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="0">
-        <v>0</v>
-      </c>
-      <c r="B62" s="0">
-        <v>0</v>
-      </c>
-      <c r="C62" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="0">
-        <v>0</v>
-      </c>
-      <c r="B63" s="0">
-        <v>0</v>
-      </c>
-      <c r="C63" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="0">
-        <v>0</v>
-      </c>
-      <c r="B64" s="0">
-        <v>0</v>
-      </c>
-      <c r="C64" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="0">
-        <v>0</v>
-      </c>
-      <c r="B65" s="0">
-        <v>0</v>
-      </c>
-      <c r="C65" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="0">
-        <v>0</v>
-      </c>
-      <c r="B66" s="0">
-        <v>0</v>
-      </c>
-      <c r="C66" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="0">
-        <v>0</v>
-      </c>
-      <c r="B67" s="0">
-        <v>0</v>
-      </c>
-      <c r="C67" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="0">
-        <v>0</v>
-      </c>
-      <c r="B68" s="0">
-        <v>0</v>
-      </c>
-      <c r="C68" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="0">
-        <v>0</v>
-      </c>
-      <c r="B69" s="0">
-        <v>0</v>
-      </c>
-      <c r="C69" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="0">
-        <v>0</v>
-      </c>
-      <c r="B70" s="0">
-        <v>0</v>
-      </c>
-      <c r="C70" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="0">
-        <v>0</v>
-      </c>
-      <c r="B71" s="0">
-        <v>0</v>
-      </c>
-      <c r="C71" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="0">
-        <v>0</v>
-      </c>
-      <c r="B72" s="0">
-        <v>0</v>
-      </c>
-      <c r="C72" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grafics d'origen energia, decisió energia i balanç economic
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -54,7 +54,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -122,530 +122,530 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>3489</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>2788</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>2807</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>769.35000000000014</v>
+        <v>3489</v>
       </c>
       <c r="B7" s="0">
-        <v>2061.8949999999991</v>
+        <v>2788</v>
       </c>
       <c r="C7" s="0">
-        <v>2227.2549999999992</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>10928.412999999993</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B8" s="0">
-        <v>6145.0419999999995</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C8" s="0">
-        <v>6425.9440000000004</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>6190.8819999999969</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B9" s="0">
-        <v>3433.9150000000004</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C9" s="0">
-        <v>4066.0949999999993</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>4529.7630000000008</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B10" s="0">
-        <v>2226.753999999999</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C10" s="0">
-        <v>2279.1679999999992</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>3586</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B11" s="0">
-        <v>2166</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C11" s="0">
-        <v>1995</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>1680.8300000000006</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>2365.848</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>2592.3199999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>10898.198999999999</v>
+        <v>3586</v>
       </c>
       <c r="B13" s="0">
-        <v>6496.1960000000036</v>
+        <v>2166</v>
       </c>
       <c r="C13" s="0">
-        <v>6838.2979999999998</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>6418.5089999999991</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B14" s="0">
-        <v>3538.2750000000015</v>
+        <v>2365.848</v>
       </c>
       <c r="C14" s="0">
-        <v>4137.1259999999975</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>4330.2969999999987</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B15" s="0">
-        <v>2277.2980000000002</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C15" s="0">
-        <v>2393.0169999999994</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>1373.362499999999</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B16" s="0">
-        <v>974.58799999999962</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C16" s="0">
-        <v>904.50499999999965</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>2226.7299999999991</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B17" s="0">
-        <v>1618.7199999999998</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>1595.3999999999992</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>11257.601999999997</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>5283.1869999999981</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>5273.3289999999988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>6446.7100000000028</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B19" s="0">
-        <v>2889.52</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C19" s="0">
-        <v>3212.8600000000006</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4436.0550000000012</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B20" s="0">
-        <v>1788.8079999999998</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1895.6379999999997</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1437.6405000000002</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B21" s="0">
-        <v>1305.6855000000005</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C21" s="0">
-        <v>1296.9269999999997</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2168.4419999999991</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B22" s="0">
-        <v>1919.04</v>
+        <v>2889.52</v>
       </c>
       <c r="C22" s="0">
-        <v>1950.3590000000004</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>9275.2019999999975</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B23" s="0">
-        <v>5731.1030000000019</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>5661.070999999999</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>5620.2959999999975</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>3200.3049999999994</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>3448.8949999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>3701.6649999999995</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B25" s="0">
-        <v>1943.5560000000007</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C25" s="0">
-        <v>1983.7219999999991</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>1512.3250000000003</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B26" s="0">
-        <v>1711.5965000000003</v>
+        <v>1919.04</v>
       </c>
       <c r="C26" s="0">
-        <v>1658.5349999999992</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1903.3499999999999</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B27" s="0">
-        <v>1415.1059999999993</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C27" s="0">
-        <v>1425.0379999999998</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>16518.094000000001</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>10803.777</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C28" s="0">
-        <v>10427.597999999998</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>5041.8729999999978</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B29" s="0">
-        <v>3122.7190000000005</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C29" s="0">
-        <v>3308.4050000000007</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>4795.8240000000023</v>
+        <v>0</v>
       </c>
       <c r="B30" s="0">
-        <v>2852.4750000000004</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>2852.4190000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>5059.6164999999946</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B31" s="0">
-        <v>3905.7699999999977</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C31" s="0">
-        <v>3782.1229999999991</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1969.172</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B32" s="0">
-        <v>892.43800000000022</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C32" s="0">
-        <v>945.06500000000028</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>26598.50299999999</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B33" s="0">
-        <v>14668.986999999999</v>
+        <v>10803.777</v>
       </c>
       <c r="C33" s="0">
-        <v>14325.897999999994</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5868.4619999999932</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B34" s="0">
-        <v>3155.5130000000022</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C34" s="0">
-        <v>3470.2359999999999</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>8294.1510000000035</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B35" s="0">
-        <v>4466.217999999998</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C35" s="0">
-        <v>4292.9000000000015</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5346.5099999999984</v>
+        <v>5.8399999999996908</v>
       </c>
       <c r="B36" s="0">
-        <v>4057.3584999999989</v>
+        <v>133.69000000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>4199.5489999999991</v>
+        <v>121.76000000000067</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>1541.1400000000006</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B37" s="0">
-        <v>774.31000000000063</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C37" s="0">
-        <v>781.94999999999982</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>23306.753000000026</v>
+        <v>1969.172</v>
       </c>
       <c r="B38" s="0">
-        <v>14927.280000000004</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C38" s="0">
-        <v>14929.637999999992</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>5499.7400000000034</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B39" s="0">
-        <v>3429.6760000000004</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>3680.5840000000017</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>7589.8439999999946</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B40" s="0">
-        <v>4775.7479999999987</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C40" s="0">
-        <v>4709.6369999999997</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>3887.4975000000031</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B41" s="0">
-        <v>2863.0859999999971</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>3005.5939999999991</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>2235.9100000000017</v>
+        <v>0</v>
       </c>
       <c r="B42" s="0">
-        <v>1762.1320000000005</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>1902.9730000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>16759.309999999994</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B43" s="0">
-        <v>9248.1730000000025</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C43" s="0">
-        <v>9299.146999999999</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>4869.9800000000023</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B44" s="0">
-        <v>2704.0450000000005</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C44" s="0">
-        <v>2941.7550000000001</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>5089.1450000000059</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B45" s="0">
-        <v>2495.0159999999996</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C45" s="0">
-        <v>2607.3530000000005</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>3381.9580000000005</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B46" s="0">
-        <v>2380.5339999999983</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>2428.5495000000019</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>2284.5360000000001</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B47" s="0">
-        <v>1891.0830000000001</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C47" s="0">
-        <v>2068.4569999999999</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>12252.739999999998</v>
+        <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>6782.1049999999932</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>6758.3839999999964</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>4328.6750000000002</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B49" s="0">
-        <v>2233.5149999999994</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C49" s="0">
-        <v>2605.3999999999987</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>3628.4829999999993</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B50" s="0">
-        <v>1841.2869999999996</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C50" s="0">
-        <v>1956.3139999999999</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>0</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B51" s="0">
-        <v>0</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C51" s="0">
-        <v>0</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>0</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B52" s="0">
-        <v>0</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C52" s="0">
-        <v>0</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>0</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B53" s="0">
-        <v>0</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>0</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="54">
@@ -661,57 +661,57 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>0</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B55" s="0">
-        <v>0</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C55" s="0">
-        <v>0</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>0</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B56" s="0">
-        <v>0</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C56" s="0">
-        <v>0</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>0</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B57" s="0">
-        <v>0</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C57" s="0">
-        <v>0</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>0</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B58" s="0">
-        <v>0</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C58" s="0">
-        <v>0</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>0</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B59" s="0">
-        <v>0</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>0</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="60">
@@ -722,6 +722,138 @@
         <v>0</v>
       </c>
       <c r="C60" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>0</v>
+      </c>
+      <c r="B61" s="0">
+        <v>0</v>
+      </c>
+      <c r="C61" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>0</v>
+      </c>
+      <c r="B62" s="0">
+        <v>0</v>
+      </c>
+      <c r="C62" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>0</v>
+      </c>
+      <c r="B63" s="0">
+        <v>0</v>
+      </c>
+      <c r="C63" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>0</v>
+      </c>
+      <c r="B64" s="0">
+        <v>0</v>
+      </c>
+      <c r="C64" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>0</v>
+      </c>
+      <c r="B65" s="0">
+        <v>0</v>
+      </c>
+      <c r="C65" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>0</v>
+      </c>
+      <c r="B66" s="0">
+        <v>0</v>
+      </c>
+      <c r="C66" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>0</v>
+      </c>
+      <c r="B67" s="0">
+        <v>0</v>
+      </c>
+      <c r="C67" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>0</v>
+      </c>
+      <c r="B68" s="0">
+        <v>0</v>
+      </c>
+      <c r="C68" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>0</v>
+      </c>
+      <c r="B69" s="0">
+        <v>0</v>
+      </c>
+      <c r="C69" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>0</v>
+      </c>
+      <c r="B70" s="0">
+        <v>0</v>
+      </c>
+      <c r="C70" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>0</v>
+      </c>
+      <c r="B71" s="0">
+        <v>0</v>
+      </c>
+      <c r="C71" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>0</v>
+      </c>
+      <c r="B72" s="0">
+        <v>0</v>
+      </c>
+      <c r="C72" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Signals for VM visualization
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -6,9 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -52,7 +51,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
@@ -60,9 +59,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Correcció error pics consum
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -6,8 +6,9 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
@@ -51,7 +52,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
@@ -59,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="9.5546875" customWidth="true"/>
+    <col min="2" max="2" width="9.5546875" customWidth="true"/>
+    <col min="3" max="3" width="9.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Some flaws of POR calculation and CE member selection
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,53 +60,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>2104</v>
+        <v>9235</v>
       </c>
       <c r="B1" s="0">
-        <v>2515</v>
+        <v>7162</v>
       </c>
       <c r="C1" s="0">
-        <v>2611</v>
+        <v>7077</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>886.08300000000008</v>
+        <v>6668</v>
       </c>
       <c r="B2" s="0">
-        <v>1925.7290000000005</v>
+        <v>2856</v>
       </c>
       <c r="C2" s="0">
-        <v>2129.4700000000003</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11543.705000000004</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B3" s="0">
-        <v>6488.0490000000018</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C3" s="0">
-        <v>6737.002000000004</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6659.7100000000019</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B4" s="0">
-        <v>3682.746000000001</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C4" s="0">
-        <v>4209.5439999999999</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="5">
@@ -133,46 +133,46 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>8467</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>6405</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>5513</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>2471</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="11">
@@ -199,46 +199,46 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>9386</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>6289</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>6385</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>5370</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>2316</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2365.848</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="17">
@@ -265,46 +265,46 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>7933</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>4609</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4364</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1440</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="23">
@@ -331,46 +331,46 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>10566</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>7921</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>8019</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>5873</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>2606</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1919.04</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="29">
@@ -397,46 +397,46 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>14563</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>9290</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>9047</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>6580</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>3214</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>10803.777</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="35">
@@ -463,46 +463,46 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>22846</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>13406</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>11278</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>8977</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>3985</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>1969.172</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="41">
@@ -529,46 +529,46 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>13791</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>13088</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>11657</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>8247</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>4344</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="47">
@@ -595,46 +595,46 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>9795</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>9224</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>8784</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>7327</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>3234</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="53">
@@ -661,46 +661,46 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>9961</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>8720</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>8305</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>5831</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>2479</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="59">

</xml_diff>

<commit_message>
Configuration of 3 EC consumption profiles and PVGenerationFactor fixed
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,53 +60,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="true"/>
-    <col min="2" max="2" width="9.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>2104</v>
+        <v>9235</v>
       </c>
       <c r="B1" s="0">
-        <v>2515</v>
+        <v>7162</v>
       </c>
       <c r="C1" s="0">
-        <v>2611</v>
+        <v>7077</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>886.08300000000008</v>
+        <v>6668</v>
       </c>
       <c r="B2" s="0">
-        <v>1925.7290000000005</v>
+        <v>2856</v>
       </c>
       <c r="C2" s="0">
-        <v>2129.4700000000003</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11543.705000000004</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B3" s="0">
-        <v>6488.0490000000018</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C3" s="0">
-        <v>6737.002000000004</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6659.7100000000019</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B4" s="0">
-        <v>3682.746000000001</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C4" s="0">
-        <v>4209.5439999999999</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="5">
@@ -133,46 +133,46 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>8467</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>6405</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>5513</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>2471</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="11">
@@ -199,46 +199,46 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>9386</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>6289</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>6385</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>5370</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>2316</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2365.848</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="17">
@@ -265,46 +265,46 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>7933</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>4609</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4364</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1440</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="23">
@@ -331,46 +331,46 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>10566</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>7921</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>8019</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>5873</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>2606</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1919.04</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="29">
@@ -397,46 +397,46 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>14563</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>9290</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>9047</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>6580</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>3214</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>10803.777</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="35">
@@ -463,46 +463,46 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>22846</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>13406</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>11278</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>8977</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>3985</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>1969.172</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="41">
@@ -529,46 +529,46 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>13791</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>13088</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>11657</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>8247</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>4344</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="47">
@@ -595,46 +595,46 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>9795</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>9224</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>8784</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>7327</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>3234</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="53">
@@ -661,46 +661,46 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>9961</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>8720</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>8305</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>5831</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>2479</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="59">

</xml_diff>

<commit_message>
Canvis funcio consum mitjà diari
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -67,46 +67,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>2104</v>
+        <v>9235</v>
       </c>
       <c r="B1" s="0">
-        <v>2515</v>
+        <v>7162</v>
       </c>
       <c r="C1" s="0">
-        <v>2611</v>
+        <v>7077</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>886.08300000000008</v>
+        <v>6668</v>
       </c>
       <c r="B2" s="0">
-        <v>1925.7290000000005</v>
+        <v>2856</v>
       </c>
       <c r="C2" s="0">
-        <v>2129.4700000000003</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11543.705000000004</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B3" s="0">
-        <v>6488.0490000000018</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C3" s="0">
-        <v>6737.002000000004</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6659.7100000000019</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B4" s="0">
-        <v>3682.746000000001</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C4" s="0">
-        <v>4209.5439999999999</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="5">
@@ -133,46 +133,46 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>8467</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>6405</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>6598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>5513</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>2471</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="11">
@@ -199,46 +199,46 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>9386</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>6289</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>6385</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>5370</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>2316</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2365.848</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="17">
@@ -265,46 +265,46 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>7933</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>4609</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4364</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1440</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="23">
@@ -331,46 +331,46 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>10566</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>7921</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>8019</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>5873</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>2606</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1919.04</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="29">
@@ -397,46 +397,46 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>14563</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>9290</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>9047</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>6580</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>3214</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>10803.777</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="35">
@@ -463,46 +463,46 @@
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>22846</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>13406</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>11278</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>8977</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>3985</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>1969.172</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="41">
@@ -529,46 +529,46 @@
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>13791</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>13088</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>11657</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>8247</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>4344</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="47">
@@ -595,46 +595,46 @@
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>9795</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>9224</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>8784</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>7327</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>3234</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="53">
@@ -661,46 +661,46 @@
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>9961</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>8720</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>8305</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>5831</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>2479</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="59">

</xml_diff>

<commit_message>
Code cleaning, name changing, and EC consumption profile definition
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -122,13 +122,13 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11543.705000000004</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B6" s="0">
-        <v>6488.0490000000018</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C6" s="0">
-        <v>6737.002000000004</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="7">
@@ -188,13 +188,13 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>10928.412999999993</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B12" s="0">
-        <v>6145.0419999999995</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C12" s="0">
-        <v>6425.9440000000004</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="13">
@@ -254,13 +254,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>10898.198999999999</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B18" s="0">
-        <v>6496.1960000000036</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C18" s="0">
-        <v>6838.2979999999998</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="19">
@@ -320,13 +320,13 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>11257.601999999997</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B24" s="0">
-        <v>5283.1869999999981</v>
+        <v>2889.52</v>
       </c>
       <c r="C24" s="0">
-        <v>5273.3289999999988</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="25">
@@ -386,13 +386,13 @@
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>9275.2019999999975</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B30" s="0">
-        <v>5731.1030000000019</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C30" s="0">
-        <v>5661.070999999999</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="31">
@@ -452,13 +452,13 @@
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>16518.094000000001</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B36" s="0">
-        <v>10803.777</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>10427.597999999998</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="37">
@@ -518,13 +518,13 @@
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>26598.50299999999</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B42" s="0">
-        <v>14668.986999999999</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C42" s="0">
-        <v>14325.897999999994</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="43">
@@ -584,13 +584,13 @@
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>23306.753000000026</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B48" s="0">
-        <v>14927.280000000004</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C48" s="0">
-        <v>14929.637999999992</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="49">
@@ -650,13 +650,13 @@
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>16759.309999999994</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B54" s="0">
-        <v>9248.1730000000025</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C54" s="0">
-        <v>9299.146999999999</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="55">
@@ -716,13 +716,13 @@
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>12252.739999999998</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B60" s="0">
-        <v>6782.1049999999932</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C60" s="0">
-        <v>6758.3839999999964</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
Canvis funcions de cost
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,9 +60,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="11.5546875" customWidth="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="true"/>
+    <col min="3" max="3" width="9.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Plots for balance service providing scenario updated
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
     <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>26216.599999999991</v>
+        <v>2104</v>
       </c>
       <c r="B1" s="0">
-        <v>23176.999999999996</v>
+        <v>2515</v>
       </c>
       <c r="C1" s="0">
-        <v>22943.100000000002</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6668</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B2" s="0">
-        <v>2856</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C2" s="0">
-        <v>2973</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2104</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B3" s="0">
-        <v>2515</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C3" s="0">
-        <v>2611</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3637</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B4" s="0">
-        <v>5012</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>5175</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>886.08300000000008</v>
+        <v>4494.0480000000007</v>
       </c>
       <c r="B5" s="0">
-        <v>1925.7290000000005</v>
+        <v>2247.5009999999997</v>
       </c>
       <c r="C5" s="0">
-        <v>2129.4700000000003</v>
+        <v>2209.3029999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6659.7100000000019</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>3682.746000000001</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>4209.5439999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24469.299999999992</v>
+        <v>3489</v>
       </c>
       <c r="B7" s="0">
-        <v>21674.298999999999</v>
+        <v>2788</v>
       </c>
       <c r="C7" s="0">
-        <v>21170.699999999997</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5513</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B8" s="0">
-        <v>2471</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C8" s="0">
-        <v>2556</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>3489</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B9" s="0">
-        <v>2788</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C9" s="0">
-        <v>2807</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>3298</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B10" s="0">
-        <v>4467</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C10" s="0">
-        <v>4646</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>769.35000000000014</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B11" s="0">
-        <v>2061.8949999999991</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C11" s="0">
-        <v>2227.2549999999992</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>6190.8819999999969</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>3433.9150000000004</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>4066.0949999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24606.971999999965</v>
+        <v>3586</v>
       </c>
       <c r="B13" s="0">
-        <v>20376.971999999998</v>
+        <v>2166</v>
       </c>
       <c r="C13" s="0">
-        <v>20264.103999999999</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>5370</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B14" s="0">
-        <v>2316</v>
+        <v>2365.848</v>
       </c>
       <c r="C14" s="0">
-        <v>2309</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>3586</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B15" s="0">
-        <v>2166</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C15" s="0">
-        <v>1995</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>2963</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B16" s="0">
-        <v>3986</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C16" s="0">
-        <v>3946</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1680.8300000000006</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B17" s="0">
-        <v>2365.848</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>2592.3199999999993</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>6418.5089999999991</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>3538.2750000000015</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>4137.1259999999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25596.69999999999</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B19" s="0">
-        <v>14632.499999999998</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C19" s="0">
-        <v>14228.300000000005</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4364</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B20" s="0">
-        <v>1440</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1579</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1373.362499999999</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B21" s="0">
-        <v>974.58799999999962</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C21" s="0">
-        <v>904.50499999999965</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2781</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B22" s="0">
-        <v>2733</v>
+        <v>2889.52</v>
       </c>
       <c r="C22" s="0">
-        <v>2582</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>2226.7299999999991</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B23" s="0">
-        <v>1618.7199999999998</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1595.3999999999992</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>6446.7100000000028</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>2889.52</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>3212.8600000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25326.990247422673</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B25" s="0">
-        <v>18115.577752577326</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C25" s="0">
-        <v>17133.401000000002</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>5873</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B26" s="0">
-        <v>2606</v>
+        <v>1919.04</v>
       </c>
       <c r="C26" s="0">
-        <v>2656</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1437.6405000000002</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B27" s="0">
-        <v>1305.6855000000005</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C27" s="0">
-        <v>1296.9269999999997</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>2865</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>5073</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C28" s="0">
-        <v>4456</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>2168.4419999999991</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B29" s="0">
-        <v>1919.04</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C29" s="0">
-        <v>1950.3590000000004</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>5620.2959999999975</v>
+        <v>0</v>
       </c>
       <c r="B30" s="0">
-        <v>3200.3049999999994</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>3448.8949999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25868.700000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B31" s="0">
-        <v>20778.599999999991</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C31" s="0">
-        <v>19379.200000000012</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>6580</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B32" s="0">
-        <v>3214</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C32" s="0">
-        <v>3375</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1512.3250000000003</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B33" s="0">
-        <v>1711.5965000000003</v>
+        <v>10803.777</v>
       </c>
       <c r="C33" s="0">
-        <v>1658.5349999999992</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>3529</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B34" s="0">
-        <v>6042</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C34" s="0">
-        <v>5353</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1903.3499999999999</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B35" s="0">
-        <v>1415.1059999999993</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C35" s="0">
-        <v>1425.0379999999998</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5041.8729999999978</v>
+        <v>5.8399999999996908</v>
       </c>
       <c r="B36" s="0">
-        <v>3122.7190000000005</v>
+        <v>133.69000000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>3308.4050000000007</v>
+        <v>121.76000000000067</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>31211.599999999955</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B37" s="0">
-        <v>22784.5</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C37" s="0">
-        <v>20634.899999999991</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>8977</v>
+        <v>1969.172</v>
       </c>
       <c r="B38" s="0">
-        <v>3985</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C38" s="0">
-        <v>4141</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>5059.6164999999946</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B39" s="0">
-        <v>3905.7699999999977</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>3782.1229999999991</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>6625</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B40" s="0">
-        <v>7274</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C40" s="0">
-        <v>6539</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1969.172</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B41" s="0">
-        <v>892.43800000000022</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>945.06500000000028</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>5868.4619999999932</v>
+        <v>0</v>
       </c>
       <c r="B42" s="0">
-        <v>3155.5130000000022</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>3470.2359999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>25209.899999999987</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B43" s="0">
-        <v>20057.599999999999</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C43" s="0">
-        <v>18162.5</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>8247</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B44" s="0">
-        <v>4344</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C44" s="0">
-        <v>4509</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>5346.5099999999984</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B45" s="0">
-        <v>4057.3584999999989</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C45" s="0">
-        <v>4199.5489999999991</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>6528</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B46" s="0">
-        <v>7836</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>6956</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1541.1400000000006</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B47" s="0">
-        <v>774.31000000000063</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C47" s="0">
-        <v>781.94999999999982</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>5499.7400000000034</v>
+        <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>3429.6760000000004</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>3680.5840000000017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>39587.899999999943</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B49" s="0">
-        <v>14817.300000000005</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C49" s="0">
-        <v>14851.200000000012</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>7327</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B50" s="0">
-        <v>3234</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C50" s="0">
-        <v>3381</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>3887.4975000000031</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B51" s="0">
-        <v>2863.0859999999971</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C51" s="0">
-        <v>3005.5939999999991</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>5609</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B52" s="0">
-        <v>5904</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C52" s="0">
-        <v>5267</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>2235.9100000000017</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B53" s="0">
-        <v>1762.1320000000005</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>1902.9730000000004</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>4869.9800000000023</v>
+        <v>0</v>
       </c>
       <c r="B54" s="0">
-        <v>2704.0450000000005</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0">
-        <v>2941.7550000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>37817.099999999969</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B55" s="0">
-        <v>14558.898999999996</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C55" s="0">
-        <v>14776.000000000007</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>5831</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B56" s="0">
-        <v>2479</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C56" s="0">
-        <v>2583</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>3381.9580000000005</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B57" s="0">
-        <v>2380.5339999999983</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C57" s="0">
-        <v>2428.5495000000019</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4039</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B58" s="0">
-        <v>4239</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C58" s="0">
-        <v>3796</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>2284.5360000000001</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B59" s="0">
-        <v>1891.0830000000001</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>2068.4569999999999</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>4328.6750000000002</v>
+        <v>0</v>
       </c>
       <c r="B60" s="0">
-        <v>2233.5149999999994</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>2605.3999999999987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
New output files and some troubleshooting
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>26216.599999999991</v>
+        <v>2104</v>
       </c>
       <c r="B1" s="0">
-        <v>23176.999999999996</v>
+        <v>2515</v>
       </c>
       <c r="C1" s="0">
-        <v>22943.100000000002</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6668</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B2" s="0">
-        <v>2856</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C2" s="0">
-        <v>2973</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2104</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B3" s="0">
-        <v>2515</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C3" s="0">
-        <v>2611</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3637</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B4" s="0">
-        <v>5012</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>5175</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>886.08300000000008</v>
+        <v>4494.0480000000007</v>
       </c>
       <c r="B5" s="0">
-        <v>1925.7290000000005</v>
+        <v>2247.5009999999997</v>
       </c>
       <c r="C5" s="0">
-        <v>2129.4700000000003</v>
+        <v>2209.3029999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6659.7100000000019</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>3682.746000000001</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>4209.5439999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24469.299999999992</v>
+        <v>3489</v>
       </c>
       <c r="B7" s="0">
-        <v>21674.298999999999</v>
+        <v>2788</v>
       </c>
       <c r="C7" s="0">
-        <v>21170.699999999997</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5513</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B8" s="0">
-        <v>2471</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C8" s="0">
-        <v>2556</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>3489</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B9" s="0">
-        <v>2788</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C9" s="0">
-        <v>2807</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>3298</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B10" s="0">
-        <v>4467</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C10" s="0">
-        <v>4646</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>769.35000000000014</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B11" s="0">
-        <v>2061.8949999999991</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C11" s="0">
-        <v>2227.2549999999992</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>6190.8819999999969</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>3433.9150000000004</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>4066.0949999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24606.971999999965</v>
+        <v>3586</v>
       </c>
       <c r="B13" s="0">
-        <v>20376.971999999998</v>
+        <v>2166</v>
       </c>
       <c r="C13" s="0">
-        <v>20264.103999999999</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>5370</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B14" s="0">
-        <v>2316</v>
+        <v>2365.848</v>
       </c>
       <c r="C14" s="0">
-        <v>2309</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>3586</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B15" s="0">
-        <v>2166</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C15" s="0">
-        <v>1995</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>2963</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B16" s="0">
-        <v>3986</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C16" s="0">
-        <v>3946</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1680.8300000000006</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B17" s="0">
-        <v>2365.848</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>2592.3199999999993</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>6418.5089999999991</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>3538.2750000000015</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>4137.1259999999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25596.69999999999</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B19" s="0">
-        <v>14632.499999999998</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C19" s="0">
-        <v>14228.300000000005</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4364</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B20" s="0">
-        <v>1440</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1579</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1373.362499999999</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B21" s="0">
-        <v>974.58799999999962</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C21" s="0">
-        <v>904.50499999999965</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2781</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B22" s="0">
-        <v>2733</v>
+        <v>2889.52</v>
       </c>
       <c r="C22" s="0">
-        <v>2582</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>2226.7299999999991</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B23" s="0">
-        <v>1618.7199999999998</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1595.3999999999992</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>6446.7100000000028</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>2889.52</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>3212.8600000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25326.990247422673</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B25" s="0">
-        <v>18115.577752577326</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C25" s="0">
-        <v>17133.401000000002</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>5873</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B26" s="0">
-        <v>2606</v>
+        <v>1919.04</v>
       </c>
       <c r="C26" s="0">
-        <v>2656</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1437.6405000000002</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B27" s="0">
-        <v>1305.6855000000005</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C27" s="0">
-        <v>1296.9269999999997</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>2865</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>5073</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C28" s="0">
-        <v>4456</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>2168.4419999999991</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B29" s="0">
-        <v>1919.04</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C29" s="0">
-        <v>1950.3590000000004</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>5620.2959999999975</v>
+        <v>0</v>
       </c>
       <c r="B30" s="0">
-        <v>3200.3049999999994</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>3448.8949999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25868.700000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B31" s="0">
-        <v>20778.599999999991</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C31" s="0">
-        <v>19379.200000000012</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>6580</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B32" s="0">
-        <v>3214</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C32" s="0">
-        <v>3375</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1512.3250000000003</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B33" s="0">
-        <v>1711.5965000000003</v>
+        <v>10803.777</v>
       </c>
       <c r="C33" s="0">
-        <v>1658.5349999999992</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>3529</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B34" s="0">
-        <v>6042</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C34" s="0">
-        <v>5353</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1903.3499999999999</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B35" s="0">
-        <v>1415.1059999999993</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C35" s="0">
-        <v>1425.0379999999998</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5041.8729999999978</v>
+        <v>5.8399999999996908</v>
       </c>
       <c r="B36" s="0">
-        <v>3122.7190000000005</v>
+        <v>133.69000000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>3308.4050000000007</v>
+        <v>121.76000000000067</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>31211.599999999955</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B37" s="0">
-        <v>22784.5</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C37" s="0">
-        <v>20634.899999999991</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>8977</v>
+        <v>1969.172</v>
       </c>
       <c r="B38" s="0">
-        <v>3985</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C38" s="0">
-        <v>4141</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>5059.6164999999946</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B39" s="0">
-        <v>3905.7699999999977</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>3782.1229999999991</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>6625</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B40" s="0">
-        <v>7274</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C40" s="0">
-        <v>6539</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1969.172</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B41" s="0">
-        <v>892.43800000000022</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>945.06500000000028</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>5868.4619999999932</v>
+        <v>0</v>
       </c>
       <c r="B42" s="0">
-        <v>3155.5130000000022</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>3470.2359999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>25209.899999999987</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B43" s="0">
-        <v>20057.599999999999</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C43" s="0">
-        <v>18162.5</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>8247</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B44" s="0">
-        <v>4344</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C44" s="0">
-        <v>4509</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>5346.5099999999984</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B45" s="0">
-        <v>4057.3584999999989</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C45" s="0">
-        <v>4199.5489999999991</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>6528</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B46" s="0">
-        <v>7836</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>6956</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1541.1400000000006</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B47" s="0">
-        <v>774.31000000000063</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C47" s="0">
-        <v>781.94999999999982</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>5499.7400000000034</v>
+        <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>3429.6760000000004</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>3680.5840000000017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>39587.899999999943</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B49" s="0">
-        <v>14817.300000000005</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C49" s="0">
-        <v>14851.200000000012</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>7327</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B50" s="0">
-        <v>3234</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C50" s="0">
-        <v>3381</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>3887.4975000000031</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B51" s="0">
-        <v>2863.0859999999971</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C51" s="0">
-        <v>3005.5939999999991</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>5609</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B52" s="0">
-        <v>5904</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C52" s="0">
-        <v>5267</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>2235.9100000000017</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B53" s="0">
-        <v>1762.1320000000005</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>1902.9730000000004</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>4869.9800000000023</v>
+        <v>0</v>
       </c>
       <c r="B54" s="0">
-        <v>2704.0450000000005</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0">
-        <v>2941.7550000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>37817.099999999969</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B55" s="0">
-        <v>14558.898999999996</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C55" s="0">
-        <v>14776.000000000007</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>5831</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B56" s="0">
-        <v>2479</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C56" s="0">
-        <v>2583</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>3381.9580000000005</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B57" s="0">
-        <v>2380.5339999999983</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C57" s="0">
-        <v>2428.5495000000019</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4039</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B58" s="0">
-        <v>4239</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C58" s="0">
-        <v>3796</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>2284.5360000000001</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B59" s="0">
-        <v>1891.0830000000001</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>2068.4569999999999</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>4328.6750000000002</v>
+        <v>0</v>
       </c>
       <c r="B60" s="0">
-        <v>2233.5149999999994</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>2605.3999999999987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
ANFIS RNN ARIMA comparison
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" customWidth="true"/>
-    <col min="3" max="3" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="11.5546875" customWidth="true"/>
+    <col min="2" max="2" width="11.5546875" customWidth="true"/>
+    <col min="3" max="3" width="9.5546875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>2104</v>
+        <v>26216.599999999991</v>
       </c>
       <c r="B1" s="0">
-        <v>2515</v>
+        <v>23176.999999999996</v>
       </c>
       <c r="C1" s="0">
-        <v>2611</v>
+        <v>22943.100000000002</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>886.08300000000008</v>
+        <v>6668</v>
       </c>
       <c r="B2" s="0">
-        <v>1925.7290000000005</v>
+        <v>2856</v>
       </c>
       <c r="C2" s="0">
-        <v>2129.4700000000003</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11543.705000000004</v>
+        <v>2104</v>
       </c>
       <c r="B3" s="0">
-        <v>6488.0490000000018</v>
+        <v>2515</v>
       </c>
       <c r="C3" s="0">
-        <v>6737.002000000004</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6659.7100000000019</v>
+        <v>3637</v>
       </c>
       <c r="B4" s="0">
-        <v>3682.746000000001</v>
+        <v>5012</v>
       </c>
       <c r="C4" s="0">
-        <v>4209.5439999999999</v>
+        <v>5175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4494.0480000000007</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B5" s="0">
-        <v>2247.5009999999997</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C5" s="0">
-        <v>2209.3029999999999</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>24469.299999999992</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>21674.298999999999</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>21170.699999999997</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>5513</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>2471</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>3489</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>2788</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>3298</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>4467</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>4646</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>4529.7630000000008</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B11" s="0">
-        <v>2226.753999999999</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C11" s="0">
-        <v>2279.1679999999992</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>24606.971999999965</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>20376.971999999998</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>20264.103999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>5370</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>2316</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>3586</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2166</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>2963</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>3986</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>4330.2969999999987</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B17" s="0">
-        <v>2277.2980000000002</v>
+        <v>2365.848</v>
       </c>
       <c r="C17" s="0">
-        <v>2393.0169999999994</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>25596.69999999999</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>14632.499999999998</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>14228.300000000005</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4364</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1440</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>2781</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>2733</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>4436.0550000000012</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B23" s="0">
-        <v>1788.8079999999998</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1895.6379999999997</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B24" s="0">
-        <v>0</v>
+        <v>2889.52</v>
       </c>
       <c r="C24" s="0">
-        <v>0</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>25326.990247422673</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>18115.577752577326</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>17133.401000000002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>5873</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>2606</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>2865</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>5073</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>3701.6649999999995</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B29" s="0">
-        <v>1943.5560000000007</v>
+        <v>1919.04</v>
       </c>
       <c r="C29" s="0">
-        <v>1983.7219999999991</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B30" s="0">
-        <v>0</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>25868.700000000001</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>20778.599999999991</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>19379.200000000012</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>6580</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>3214</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>3529</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>6042</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>5353</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>4795.8240000000023</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B35" s="0">
-        <v>2852.4750000000004</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C35" s="0">
-        <v>2852.4190000000003</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5.8399999999996908</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B36" s="0">
-        <v>133.69000000000005</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>121.76000000000067</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>31211.599999999955</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>22784.5</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>20634.899999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>8977</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>3985</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>6625</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>7274</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>6539</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>8294.1510000000035</v>
+        <v>1969.172</v>
       </c>
       <c r="B41" s="0">
-        <v>4466.217999999998</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C41" s="0">
-        <v>4292.9000000000015</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B42" s="0">
-        <v>0</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>25209.899999999987</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>20057.599999999999</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>18162.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>8247</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>4344</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>6528</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>7836</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>7589.8439999999946</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B47" s="0">
-        <v>4775.7479999999987</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C47" s="0">
-        <v>4709.6369999999997</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B48" s="0">
-        <v>0</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>39587.899999999943</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>14817.300000000005</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>14851.200000000012</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>7327</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>3234</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>5609</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>5904</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>5267</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>5089.1450000000059</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B53" s="0">
-        <v>2495.0159999999996</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C53" s="0">
-        <v>2607.3530000000005</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B54" s="0">
-        <v>0</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C54" s="0">
-        <v>0</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>37817.099999999969</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>14558.898999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>14776.000000000007</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>5831</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>2479</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>4039</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>4239</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>3628.4829999999993</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B59" s="0">
-        <v>1841.2869999999996</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C59" s="0">
-        <v>1956.3139999999999</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B60" s="0">
-        <v>0</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C60" s="0">
-        <v>0</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
scenario basic rules fixed
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="true"/>
-    <col min="2" max="2" width="11.5546875" customWidth="true"/>
-    <col min="3" max="3" width="9.5546875" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>26216.599999999991</v>
+        <v>2104</v>
       </c>
       <c r="B1" s="0">
-        <v>23176.999999999996</v>
+        <v>2515</v>
       </c>
       <c r="C1" s="0">
-        <v>22943.100000000002</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6668</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B2" s="0">
-        <v>2856</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C2" s="0">
-        <v>2973</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2104</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B3" s="0">
-        <v>2515</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C3" s="0">
-        <v>2611</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3637</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B4" s="0">
-        <v>5012</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>5175</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>886.08300000000008</v>
+        <v>4494.0480000000007</v>
       </c>
       <c r="B5" s="0">
-        <v>1925.7290000000005</v>
+        <v>2247.5009999999997</v>
       </c>
       <c r="C5" s="0">
-        <v>2129.4700000000003</v>
+        <v>2209.3029999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6659.7100000000019</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>3682.746000000001</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>4209.5439999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24469.299999999992</v>
+        <v>3489</v>
       </c>
       <c r="B7" s="0">
-        <v>21674.298999999999</v>
+        <v>2788</v>
       </c>
       <c r="C7" s="0">
-        <v>21170.699999999997</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5513</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B8" s="0">
-        <v>2471</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C8" s="0">
-        <v>2556</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>3489</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B9" s="0">
-        <v>2788</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C9" s="0">
-        <v>2807</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>3298</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B10" s="0">
-        <v>4467</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C10" s="0">
-        <v>4646</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>769.35000000000014</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B11" s="0">
-        <v>2061.8949999999991</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C11" s="0">
-        <v>2227.2549999999992</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>6190.8819999999969</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>3433.9150000000004</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>4066.0949999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24606.971999999965</v>
+        <v>3586</v>
       </c>
       <c r="B13" s="0">
-        <v>20376.971999999998</v>
+        <v>2166</v>
       </c>
       <c r="C13" s="0">
-        <v>20264.103999999999</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>5370</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B14" s="0">
-        <v>2316</v>
+        <v>2365.848</v>
       </c>
       <c r="C14" s="0">
-        <v>2309</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>3586</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B15" s="0">
-        <v>2166</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C15" s="0">
-        <v>1995</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>2963</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B16" s="0">
-        <v>3986</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C16" s="0">
-        <v>3946</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1680.8300000000006</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B17" s="0">
-        <v>2365.848</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>2592.3199999999993</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>6418.5089999999991</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>3538.2750000000015</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>4137.1259999999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25596.69999999999</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B19" s="0">
-        <v>14632.499999999998</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C19" s="0">
-        <v>14228.300000000005</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4364</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B20" s="0">
-        <v>1440</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1579</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1373.362499999999</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B21" s="0">
-        <v>974.58799999999962</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C21" s="0">
-        <v>904.50499999999965</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2781</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B22" s="0">
-        <v>2733</v>
+        <v>2889.52</v>
       </c>
       <c r="C22" s="0">
-        <v>2582</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>2226.7299999999991</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B23" s="0">
-        <v>1618.7199999999998</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1595.3999999999992</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>6446.7100000000028</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>2889.52</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>3212.8600000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25326.990247422673</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B25" s="0">
-        <v>18115.577752577326</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C25" s="0">
-        <v>17133.401000000002</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>5873</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B26" s="0">
-        <v>2606</v>
+        <v>1919.04</v>
       </c>
       <c r="C26" s="0">
-        <v>2656</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1437.6405000000002</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B27" s="0">
-        <v>1305.6855000000005</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C27" s="0">
-        <v>1296.9269999999997</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>2865</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>5073</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C28" s="0">
-        <v>4456</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>2168.4419999999991</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B29" s="0">
-        <v>1919.04</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C29" s="0">
-        <v>1950.3590000000004</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>5620.2959999999975</v>
+        <v>0</v>
       </c>
       <c r="B30" s="0">
-        <v>3200.3049999999994</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>3448.8949999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25868.700000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B31" s="0">
-        <v>20778.599999999991</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C31" s="0">
-        <v>19379.200000000012</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>6580</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B32" s="0">
-        <v>3214</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C32" s="0">
-        <v>3375</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1512.3250000000003</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B33" s="0">
-        <v>1711.5965000000003</v>
+        <v>10803.777</v>
       </c>
       <c r="C33" s="0">
-        <v>1658.5349999999992</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>3529</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B34" s="0">
-        <v>6042</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C34" s="0">
-        <v>5353</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1903.3499999999999</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B35" s="0">
-        <v>1415.1059999999993</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C35" s="0">
-        <v>1425.0379999999998</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5041.8729999999978</v>
+        <v>5.8399999999996908</v>
       </c>
       <c r="B36" s="0">
-        <v>3122.7190000000005</v>
+        <v>133.69000000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>3308.4050000000007</v>
+        <v>121.76000000000067</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>31211.599999999955</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B37" s="0">
-        <v>22784.5</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C37" s="0">
-        <v>20634.899999999991</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>8977</v>
+        <v>1969.172</v>
       </c>
       <c r="B38" s="0">
-        <v>3985</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C38" s="0">
-        <v>4141</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>5059.6164999999946</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B39" s="0">
-        <v>3905.7699999999977</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>3782.1229999999991</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>6625</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B40" s="0">
-        <v>7274</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C40" s="0">
-        <v>6539</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1969.172</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B41" s="0">
-        <v>892.43800000000022</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>945.06500000000028</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>5868.4619999999932</v>
+        <v>0</v>
       </c>
       <c r="B42" s="0">
-        <v>3155.5130000000022</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>3470.2359999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>25209.899999999987</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B43" s="0">
-        <v>20057.599999999999</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C43" s="0">
-        <v>18162.5</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>8247</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B44" s="0">
-        <v>4344</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C44" s="0">
-        <v>4509</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>5346.5099999999984</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B45" s="0">
-        <v>4057.3584999999989</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C45" s="0">
-        <v>4199.5489999999991</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>6528</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B46" s="0">
-        <v>7836</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>6956</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1541.1400000000006</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B47" s="0">
-        <v>774.31000000000063</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C47" s="0">
-        <v>781.94999999999982</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>5499.7400000000034</v>
+        <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>3429.6760000000004</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>3680.5840000000017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>39587.899999999943</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B49" s="0">
-        <v>14817.300000000005</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C49" s="0">
-        <v>14851.200000000012</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>7327</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B50" s="0">
-        <v>3234</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C50" s="0">
-        <v>3381</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>3887.4975000000031</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B51" s="0">
-        <v>2863.0859999999971</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C51" s="0">
-        <v>3005.5939999999991</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>5609</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B52" s="0">
-        <v>5904</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C52" s="0">
-        <v>5267</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>2235.9100000000017</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B53" s="0">
-        <v>1762.1320000000005</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>1902.9730000000004</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>4869.9800000000023</v>
+        <v>0</v>
       </c>
       <c r="B54" s="0">
-        <v>2704.0450000000005</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0">
-        <v>2941.7550000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>37817.099999999969</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B55" s="0">
-        <v>14558.898999999996</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C55" s="0">
-        <v>14776.000000000007</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>5831</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B56" s="0">
-        <v>2479</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C56" s="0">
-        <v>2583</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>3381.9580000000005</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B57" s="0">
-        <v>2380.5339999999983</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C57" s="0">
-        <v>2428.5495000000019</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4039</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B58" s="0">
-        <v>4239</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C58" s="0">
-        <v>3796</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>2284.5360000000001</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B59" s="0">
-        <v>1891.0830000000001</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>2068.4569999999999</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>4328.6750000000002</v>
+        <v>0</v>
       </c>
       <c r="B60" s="0">
-        <v>2233.5149999999994</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>2605.3999999999987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
Some plots were updated
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="true"/>
-    <col min="2" max="2" width="9.7109375" customWidth="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="true"/>
+    <col min="2" max="2" width="11.7109375" customWidth="true"/>
     <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>2104</v>
+        <v>26216.599999999991</v>
       </c>
       <c r="B1" s="0">
-        <v>2515</v>
+        <v>23176.999999999996</v>
       </c>
       <c r="C1" s="0">
-        <v>2611</v>
+        <v>22943.100000000002</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>886.08300000000008</v>
+        <v>6668</v>
       </c>
       <c r="B2" s="0">
-        <v>1925.7290000000005</v>
+        <v>2856</v>
       </c>
       <c r="C2" s="0">
-        <v>2129.4700000000003</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11543.705000000004</v>
+        <v>2104</v>
       </c>
       <c r="B3" s="0">
-        <v>6488.0490000000018</v>
+        <v>2515</v>
       </c>
       <c r="C3" s="0">
-        <v>6737.002000000004</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>6659.7100000000019</v>
+        <v>3637</v>
       </c>
       <c r="B4" s="0">
-        <v>3682.746000000001</v>
+        <v>5012</v>
       </c>
       <c r="C4" s="0">
-        <v>4209.5439999999999</v>
+        <v>5175</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4494.0480000000007</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B5" s="0">
-        <v>2247.5009999999997</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C5" s="0">
-        <v>2209.3029999999999</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>3489</v>
+        <v>24469.299999999992</v>
       </c>
       <c r="B7" s="0">
-        <v>2788</v>
+        <v>21674.298999999999</v>
       </c>
       <c r="C7" s="0">
-        <v>2807</v>
+        <v>21170.699999999997</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>769.35000000000014</v>
+        <v>5513</v>
       </c>
       <c r="B8" s="0">
-        <v>2061.8949999999991</v>
+        <v>2471</v>
       </c>
       <c r="C8" s="0">
-        <v>2227.2549999999992</v>
+        <v>2556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10928.412999999993</v>
+        <v>3489</v>
       </c>
       <c r="B9" s="0">
-        <v>6145.0419999999995</v>
+        <v>2788</v>
       </c>
       <c r="C9" s="0">
-        <v>6425.9440000000004</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6190.8819999999969</v>
+        <v>3298</v>
       </c>
       <c r="B10" s="0">
-        <v>3433.9150000000004</v>
+        <v>4467</v>
       </c>
       <c r="C10" s="0">
-        <v>4066.0949999999993</v>
+        <v>4646</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>4529.7630000000008</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B11" s="0">
-        <v>2226.753999999999</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C11" s="0">
-        <v>2279.1679999999992</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>3586</v>
+        <v>24606.971999999965</v>
       </c>
       <c r="B13" s="0">
-        <v>2166</v>
+        <v>20376.971999999998</v>
       </c>
       <c r="C13" s="0">
-        <v>1995</v>
+        <v>20264.103999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1680.8300000000006</v>
+        <v>5370</v>
       </c>
       <c r="B14" s="0">
-        <v>2365.848</v>
+        <v>2316</v>
       </c>
       <c r="C14" s="0">
-        <v>2592.3199999999993</v>
+        <v>2309</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10898.198999999999</v>
+        <v>3586</v>
       </c>
       <c r="B15" s="0">
-        <v>6496.1960000000036</v>
+        <v>2166</v>
       </c>
       <c r="C15" s="0">
-        <v>6838.2979999999998</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6418.5089999999991</v>
+        <v>2963</v>
       </c>
       <c r="B16" s="0">
-        <v>3538.2750000000015</v>
+        <v>3986</v>
       </c>
       <c r="C16" s="0">
-        <v>4137.1259999999975</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>4330.2969999999987</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B17" s="0">
-        <v>2277.2980000000002</v>
+        <v>2365.848</v>
       </c>
       <c r="C17" s="0">
-        <v>2393.0169999999994</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1373.362499999999</v>
+        <v>25596.69999999999</v>
       </c>
       <c r="B19" s="0">
-        <v>974.58799999999962</v>
+        <v>14632.499999999998</v>
       </c>
       <c r="C19" s="0">
-        <v>904.50499999999965</v>
+        <v>14228.300000000005</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>2226.7299999999991</v>
+        <v>4364</v>
       </c>
       <c r="B20" s="0">
-        <v>1618.7199999999998</v>
+        <v>1440</v>
       </c>
       <c r="C20" s="0">
-        <v>1595.3999999999992</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>11257.601999999997</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B21" s="0">
-        <v>5283.1869999999981</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C21" s="0">
-        <v>5273.3289999999988</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>6446.7100000000028</v>
+        <v>2781</v>
       </c>
       <c r="B22" s="0">
-        <v>2889.52</v>
+        <v>2733</v>
       </c>
       <c r="C22" s="0">
-        <v>3212.8600000000006</v>
+        <v>2582</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>4436.0550000000012</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B23" s="0">
-        <v>1788.8079999999998</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1895.6379999999997</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>0</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B24" s="0">
-        <v>0</v>
+        <v>2889.52</v>
       </c>
       <c r="C24" s="0">
-        <v>0</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>1437.6405000000002</v>
+        <v>25326.990247422673</v>
       </c>
       <c r="B25" s="0">
-        <v>1305.6855000000005</v>
+        <v>18115.577752577326</v>
       </c>
       <c r="C25" s="0">
-        <v>1296.9269999999997</v>
+        <v>17133.401000000002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>2168.4419999999991</v>
+        <v>5873</v>
       </c>
       <c r="B26" s="0">
-        <v>1919.04</v>
+        <v>2606</v>
       </c>
       <c r="C26" s="0">
-        <v>1950.3590000000004</v>
+        <v>2656</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>9275.2019999999975</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B27" s="0">
-        <v>5731.1030000000019</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C27" s="0">
-        <v>5661.070999999999</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>5620.2959999999975</v>
+        <v>2865</v>
       </c>
       <c r="B28" s="0">
-        <v>3200.3049999999994</v>
+        <v>5073</v>
       </c>
       <c r="C28" s="0">
-        <v>3448.8949999999995</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>3701.6649999999995</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B29" s="0">
-        <v>1943.5560000000007</v>
+        <v>1919.04</v>
       </c>
       <c r="C29" s="0">
-        <v>1983.7219999999991</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>0</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B30" s="0">
-        <v>0</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C30" s="0">
-        <v>0</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>1512.3250000000003</v>
+        <v>25868.700000000001</v>
       </c>
       <c r="B31" s="0">
-        <v>1711.5965000000003</v>
+        <v>20778.599999999991</v>
       </c>
       <c r="C31" s="0">
-        <v>1658.5349999999992</v>
+        <v>19379.200000000012</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>1903.3499999999999</v>
+        <v>6580</v>
       </c>
       <c r="B32" s="0">
-        <v>1415.1059999999993</v>
+        <v>3214</v>
       </c>
       <c r="C32" s="0">
-        <v>1425.0379999999998</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>16518.094000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B33" s="0">
-        <v>10803.777</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C33" s="0">
-        <v>10427.597999999998</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>5041.8729999999978</v>
+        <v>3529</v>
       </c>
       <c r="B34" s="0">
-        <v>3122.7190000000005</v>
+        <v>6042</v>
       </c>
       <c r="C34" s="0">
-        <v>3308.4050000000007</v>
+        <v>5353</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>4795.8240000000023</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B35" s="0">
-        <v>2852.4750000000004</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C35" s="0">
-        <v>2852.4190000000003</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5.8399999999996908</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B36" s="0">
-        <v>133.69000000000005</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>121.76000000000067</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>5059.6164999999946</v>
+        <v>31211.599999999955</v>
       </c>
       <c r="B37" s="0">
-        <v>3905.7699999999977</v>
+        <v>22784.5</v>
       </c>
       <c r="C37" s="0">
-        <v>3782.1229999999991</v>
+        <v>20634.899999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>1969.172</v>
+        <v>8977</v>
       </c>
       <c r="B38" s="0">
-        <v>892.43800000000022</v>
+        <v>3985</v>
       </c>
       <c r="C38" s="0">
-        <v>945.06500000000028</v>
+        <v>4141</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>26598.50299999999</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B39" s="0">
-        <v>14668.986999999999</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C39" s="0">
-        <v>14325.897999999994</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>5868.4619999999932</v>
+        <v>6625</v>
       </c>
       <c r="B40" s="0">
-        <v>3155.5130000000022</v>
+        <v>7274</v>
       </c>
       <c r="C40" s="0">
-        <v>3470.2359999999999</v>
+        <v>6539</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>8294.1510000000035</v>
+        <v>1969.172</v>
       </c>
       <c r="B41" s="0">
-        <v>4466.217999999998</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C41" s="0">
-        <v>4292.9000000000015</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>0</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B42" s="0">
-        <v>0</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C42" s="0">
-        <v>0</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>5346.5099999999984</v>
+        <v>25209.899999999987</v>
       </c>
       <c r="B43" s="0">
-        <v>4057.3584999999989</v>
+        <v>20057.599999999999</v>
       </c>
       <c r="C43" s="0">
-        <v>4199.5489999999991</v>
+        <v>18162.5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>1541.1400000000006</v>
+        <v>8247</v>
       </c>
       <c r="B44" s="0">
-        <v>774.31000000000063</v>
+        <v>4344</v>
       </c>
       <c r="C44" s="0">
-        <v>781.94999999999982</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>23306.753000000026</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B45" s="0">
-        <v>14927.280000000004</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C45" s="0">
-        <v>14929.637999999992</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>5499.7400000000034</v>
+        <v>6528</v>
       </c>
       <c r="B46" s="0">
-        <v>3429.6760000000004</v>
+        <v>7836</v>
       </c>
       <c r="C46" s="0">
-        <v>3680.5840000000017</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>7589.8439999999946</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B47" s="0">
-        <v>4775.7479999999987</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C47" s="0">
-        <v>4709.6369999999997</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>0</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B48" s="0">
-        <v>0</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C48" s="0">
-        <v>0</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>3887.4975000000031</v>
+        <v>39587.899999999943</v>
       </c>
       <c r="B49" s="0">
-        <v>2863.0859999999971</v>
+        <v>14817.300000000005</v>
       </c>
       <c r="C49" s="0">
-        <v>3005.5939999999991</v>
+        <v>14851.200000000012</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>2235.9100000000017</v>
+        <v>7327</v>
       </c>
       <c r="B50" s="0">
-        <v>1762.1320000000005</v>
+        <v>3234</v>
       </c>
       <c r="C50" s="0">
-        <v>1902.9730000000004</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>16759.309999999994</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B51" s="0">
-        <v>9248.1730000000025</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C51" s="0">
-        <v>9299.146999999999</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>4869.9800000000023</v>
+        <v>5609</v>
       </c>
       <c r="B52" s="0">
-        <v>2704.0450000000005</v>
+        <v>5904</v>
       </c>
       <c r="C52" s="0">
-        <v>2941.7550000000001</v>
+        <v>5267</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>5089.1450000000059</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B53" s="0">
-        <v>2495.0159999999996</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C53" s="0">
-        <v>2607.3530000000005</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>0</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B54" s="0">
-        <v>0</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C54" s="0">
-        <v>0</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>3381.9580000000005</v>
+        <v>37817.099999999969</v>
       </c>
       <c r="B55" s="0">
-        <v>2380.5339999999983</v>
+        <v>14558.898999999996</v>
       </c>
       <c r="C55" s="0">
-        <v>2428.5495000000019</v>
+        <v>14776.000000000007</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>2284.5360000000001</v>
+        <v>5831</v>
       </c>
       <c r="B56" s="0">
-        <v>1891.0830000000001</v>
+        <v>2479</v>
       </c>
       <c r="C56" s="0">
-        <v>2068.4569999999999</v>
+        <v>2583</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>12252.739999999998</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B57" s="0">
-        <v>6782.1049999999932</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C57" s="0">
-        <v>6758.3839999999964</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4328.6750000000002</v>
+        <v>4039</v>
       </c>
       <c r="B58" s="0">
-        <v>2233.5149999999994</v>
+        <v>4239</v>
       </c>
       <c r="C58" s="0">
-        <v>2605.3999999999987</v>
+        <v>3796</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>3628.4829999999993</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B59" s="0">
-        <v>1841.2869999999996</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C59" s="0">
-        <v>1956.3139999999999</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>0</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B60" s="0">
-        <v>0</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C60" s="0">
-        <v>0</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="61">

</xml_diff>

<commit_message>
Slides_scripts updated after Cagliari
</commit_message>
<xml_diff>
--- a/_data/bbce2_Factures_ficticies.xlsx
+++ b/_data/bbce2_Factures_ficticies.xlsx
@@ -60,669 +60,669 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="true"/>
-    <col min="2" max="2" width="11.7109375" customWidth="true"/>
+    <col min="1" max="1" width="9.7109375" customWidth="true"/>
+    <col min="2" max="2" width="9.7109375" customWidth="true"/>
     <col min="3" max="3" width="9.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0">
-        <v>26216.599999999991</v>
+        <v>2104</v>
       </c>
       <c r="B1" s="0">
-        <v>23176.999999999996</v>
+        <v>2515</v>
       </c>
       <c r="C1" s="0">
-        <v>22943.100000000002</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6668</v>
+        <v>886.08300000000008</v>
       </c>
       <c r="B2" s="0">
-        <v>2856</v>
+        <v>1925.7290000000005</v>
       </c>
       <c r="C2" s="0">
-        <v>2973</v>
+        <v>2129.4700000000003</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2104</v>
+        <v>11543.705000000004</v>
       </c>
       <c r="B3" s="0">
-        <v>2515</v>
+        <v>6488.0490000000018</v>
       </c>
       <c r="C3" s="0">
-        <v>2611</v>
+        <v>6737.002000000004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>3637</v>
+        <v>6659.7100000000019</v>
       </c>
       <c r="B4" s="0">
-        <v>5012</v>
+        <v>3682.746000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>5175</v>
+        <v>4209.5439999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>886.08300000000008</v>
+        <v>4494.0480000000007</v>
       </c>
       <c r="B5" s="0">
-        <v>1925.7290000000005</v>
+        <v>2247.5009999999997</v>
       </c>
       <c r="C5" s="0">
-        <v>2129.4700000000003</v>
+        <v>2209.3029999999999</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6659.7100000000019</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>3682.746000000001</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>4209.5439999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24469.299999999992</v>
+        <v>3489</v>
       </c>
       <c r="B7" s="0">
-        <v>21674.298999999999</v>
+        <v>2788</v>
       </c>
       <c r="C7" s="0">
-        <v>21170.699999999997</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>5513</v>
+        <v>769.35000000000014</v>
       </c>
       <c r="B8" s="0">
-        <v>2471</v>
+        <v>2061.8949999999991</v>
       </c>
       <c r="C8" s="0">
-        <v>2556</v>
+        <v>2227.2549999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>3489</v>
+        <v>10928.412999999993</v>
       </c>
       <c r="B9" s="0">
-        <v>2788</v>
+        <v>6145.0419999999995</v>
       </c>
       <c r="C9" s="0">
-        <v>2807</v>
+        <v>6425.9440000000004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>3298</v>
+        <v>6190.8819999999969</v>
       </c>
       <c r="B10" s="0">
-        <v>4467</v>
+        <v>3433.9150000000004</v>
       </c>
       <c r="C10" s="0">
-        <v>4646</v>
+        <v>4066.0949999999993</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>769.35000000000014</v>
+        <v>4529.7630000000008</v>
       </c>
       <c r="B11" s="0">
-        <v>2061.8949999999991</v>
+        <v>2226.753999999999</v>
       </c>
       <c r="C11" s="0">
-        <v>2227.2549999999992</v>
+        <v>2279.1679999999992</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>6190.8819999999969</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>3433.9150000000004</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>4066.0949999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>24606.971999999965</v>
+        <v>3586</v>
       </c>
       <c r="B13" s="0">
-        <v>20376.971999999998</v>
+        <v>2166</v>
       </c>
       <c r="C13" s="0">
-        <v>20264.103999999999</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>5370</v>
+        <v>1680.8300000000006</v>
       </c>
       <c r="B14" s="0">
-        <v>2316</v>
+        <v>2365.848</v>
       </c>
       <c r="C14" s="0">
-        <v>2309</v>
+        <v>2592.3199999999993</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>3586</v>
+        <v>10898.198999999999</v>
       </c>
       <c r="B15" s="0">
-        <v>2166</v>
+        <v>6496.1960000000036</v>
       </c>
       <c r="C15" s="0">
-        <v>1995</v>
+        <v>6838.2979999999998</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>2963</v>
+        <v>6418.5089999999991</v>
       </c>
       <c r="B16" s="0">
-        <v>3986</v>
+        <v>3538.2750000000015</v>
       </c>
       <c r="C16" s="0">
-        <v>3946</v>
+        <v>4137.1259999999975</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>1680.8300000000006</v>
+        <v>4330.2969999999987</v>
       </c>
       <c r="B17" s="0">
-        <v>2365.848</v>
+        <v>2277.2980000000002</v>
       </c>
       <c r="C17" s="0">
-        <v>2592.3199999999993</v>
+        <v>2393.0169999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>6418.5089999999991</v>
+        <v>0</v>
       </c>
       <c r="B18" s="0">
-        <v>3538.2750000000015</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0">
-        <v>4137.1259999999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>25596.69999999999</v>
+        <v>1373.362499999999</v>
       </c>
       <c r="B19" s="0">
-        <v>14632.499999999998</v>
+        <v>974.58799999999962</v>
       </c>
       <c r="C19" s="0">
-        <v>14228.300000000005</v>
+        <v>904.50499999999965</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4364</v>
+        <v>2226.7299999999991</v>
       </c>
       <c r="B20" s="0">
-        <v>1440</v>
+        <v>1618.7199999999998</v>
       </c>
       <c r="C20" s="0">
-        <v>1579</v>
+        <v>1595.3999999999992</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1373.362499999999</v>
+        <v>11257.601999999997</v>
       </c>
       <c r="B21" s="0">
-        <v>974.58799999999962</v>
+        <v>5283.1869999999981</v>
       </c>
       <c r="C21" s="0">
-        <v>904.50499999999965</v>
+        <v>5273.3289999999988</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>2781</v>
+        <v>6446.7100000000028</v>
       </c>
       <c r="B22" s="0">
-        <v>2733</v>
+        <v>2889.52</v>
       </c>
       <c r="C22" s="0">
-        <v>2582</v>
+        <v>3212.8600000000006</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>2226.7299999999991</v>
+        <v>4436.0550000000012</v>
       </c>
       <c r="B23" s="0">
-        <v>1618.7199999999998</v>
+        <v>1788.8079999999998</v>
       </c>
       <c r="C23" s="0">
-        <v>1595.3999999999992</v>
+        <v>1895.6379999999997</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>6446.7100000000028</v>
+        <v>0</v>
       </c>
       <c r="B24" s="0">
-        <v>2889.52</v>
+        <v>0</v>
       </c>
       <c r="C24" s="0">
-        <v>3212.8600000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>25326.990247422673</v>
+        <v>1437.6405000000002</v>
       </c>
       <c r="B25" s="0">
-        <v>18115.577752577326</v>
+        <v>1305.6855000000005</v>
       </c>
       <c r="C25" s="0">
-        <v>17133.401000000002</v>
+        <v>1296.9269999999997</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>5873</v>
+        <v>2168.4419999999991</v>
       </c>
       <c r="B26" s="0">
-        <v>2606</v>
+        <v>1919.04</v>
       </c>
       <c r="C26" s="0">
-        <v>2656</v>
+        <v>1950.3590000000004</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1437.6405000000002</v>
+        <v>9275.2019999999975</v>
       </c>
       <c r="B27" s="0">
-        <v>1305.6855000000005</v>
+        <v>5731.1030000000019</v>
       </c>
       <c r="C27" s="0">
-        <v>1296.9269999999997</v>
+        <v>5661.070999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>2865</v>
+        <v>5620.2959999999975</v>
       </c>
       <c r="B28" s="0">
-        <v>5073</v>
+        <v>3200.3049999999994</v>
       </c>
       <c r="C28" s="0">
-        <v>4456</v>
+        <v>3448.8949999999995</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>2168.4419999999991</v>
+        <v>3701.6649999999995</v>
       </c>
       <c r="B29" s="0">
-        <v>1919.04</v>
+        <v>1943.5560000000007</v>
       </c>
       <c r="C29" s="0">
-        <v>1950.3590000000004</v>
+        <v>1983.7219999999991</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>5620.2959999999975</v>
+        <v>0</v>
       </c>
       <c r="B30" s="0">
-        <v>3200.3049999999994</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0">
-        <v>3448.8949999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>25868.700000000001</v>
+        <v>1512.3250000000003</v>
       </c>
       <c r="B31" s="0">
-        <v>20778.599999999991</v>
+        <v>1711.5965000000003</v>
       </c>
       <c r="C31" s="0">
-        <v>19379.200000000012</v>
+        <v>1658.5349999999992</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>6580</v>
+        <v>1903.3499999999999</v>
       </c>
       <c r="B32" s="0">
-        <v>3214</v>
+        <v>1415.1059999999993</v>
       </c>
       <c r="C32" s="0">
-        <v>3375</v>
+        <v>1425.0379999999998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>1512.3250000000003</v>
+        <v>16518.094000000001</v>
       </c>
       <c r="B33" s="0">
-        <v>1711.5965000000003</v>
+        <v>10803.777</v>
       </c>
       <c r="C33" s="0">
-        <v>1658.5349999999992</v>
+        <v>10427.597999999998</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>3529</v>
+        <v>5041.8729999999978</v>
       </c>
       <c r="B34" s="0">
-        <v>6042</v>
+        <v>3122.7190000000005</v>
       </c>
       <c r="C34" s="0">
-        <v>5353</v>
+        <v>3308.4050000000007</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>1903.3499999999999</v>
+        <v>4795.8240000000023</v>
       </c>
       <c r="B35" s="0">
-        <v>1415.1059999999993</v>
+        <v>2852.4750000000004</v>
       </c>
       <c r="C35" s="0">
-        <v>1425.0379999999998</v>
+        <v>2852.4190000000003</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>5041.8729999999978</v>
+        <v>5.8399999999996908</v>
       </c>
       <c r="B36" s="0">
-        <v>3122.7190000000005</v>
+        <v>133.69000000000005</v>
       </c>
       <c r="C36" s="0">
-        <v>3308.4050000000007</v>
+        <v>121.76000000000067</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>31211.599999999955</v>
+        <v>5059.6164999999946</v>
       </c>
       <c r="B37" s="0">
-        <v>22784.5</v>
+        <v>3905.7699999999977</v>
       </c>
       <c r="C37" s="0">
-        <v>20634.899999999991</v>
+        <v>3782.1229999999991</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>8977</v>
+        <v>1969.172</v>
       </c>
       <c r="B38" s="0">
-        <v>3985</v>
+        <v>892.43800000000022</v>
       </c>
       <c r="C38" s="0">
-        <v>4141</v>
+        <v>945.06500000000028</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>5059.6164999999946</v>
+        <v>26598.50299999999</v>
       </c>
       <c r="B39" s="0">
-        <v>3905.7699999999977</v>
+        <v>14668.986999999999</v>
       </c>
       <c r="C39" s="0">
-        <v>3782.1229999999991</v>
+        <v>14325.897999999994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>6625</v>
+        <v>5868.4619999999932</v>
       </c>
       <c r="B40" s="0">
-        <v>7274</v>
+        <v>3155.5130000000022</v>
       </c>
       <c r="C40" s="0">
-        <v>6539</v>
+        <v>3470.2359999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>1969.172</v>
+        <v>8294.1510000000035</v>
       </c>
       <c r="B41" s="0">
-        <v>892.43800000000022</v>
+        <v>4466.217999999998</v>
       </c>
       <c r="C41" s="0">
-        <v>945.06500000000028</v>
+        <v>4292.9000000000015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>5868.4619999999932</v>
+        <v>0</v>
       </c>
       <c r="B42" s="0">
-        <v>3155.5130000000022</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0">
-        <v>3470.2359999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>25209.899999999987</v>
+        <v>5346.5099999999984</v>
       </c>
       <c r="B43" s="0">
-        <v>20057.599999999999</v>
+        <v>4057.3584999999989</v>
       </c>
       <c r="C43" s="0">
-        <v>18162.5</v>
+        <v>4199.5489999999991</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>8247</v>
+        <v>1541.1400000000006</v>
       </c>
       <c r="B44" s="0">
-        <v>4344</v>
+        <v>774.31000000000063</v>
       </c>
       <c r="C44" s="0">
-        <v>4509</v>
+        <v>781.94999999999982</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>5346.5099999999984</v>
+        <v>23306.753000000026</v>
       </c>
       <c r="B45" s="0">
-        <v>4057.3584999999989</v>
+        <v>14927.280000000004</v>
       </c>
       <c r="C45" s="0">
-        <v>4199.5489999999991</v>
+        <v>14929.637999999992</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>6528</v>
+        <v>5499.7400000000034</v>
       </c>
       <c r="B46" s="0">
-        <v>7836</v>
+        <v>3429.6760000000004</v>
       </c>
       <c r="C46" s="0">
-        <v>6956</v>
+        <v>3680.5840000000017</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>1541.1400000000006</v>
+        <v>7589.8439999999946</v>
       </c>
       <c r="B47" s="0">
-        <v>774.31000000000063</v>
+        <v>4775.7479999999987</v>
       </c>
       <c r="C47" s="0">
-        <v>781.94999999999982</v>
+        <v>4709.6369999999997</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>5499.7400000000034</v>
+        <v>0</v>
       </c>
       <c r="B48" s="0">
-        <v>3429.6760000000004</v>
+        <v>0</v>
       </c>
       <c r="C48" s="0">
-        <v>3680.5840000000017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>39587.899999999943</v>
+        <v>3887.4975000000031</v>
       </c>
       <c r="B49" s="0">
-        <v>14817.300000000005</v>
+        <v>2863.0859999999971</v>
       </c>
       <c r="C49" s="0">
-        <v>14851.200000000012</v>
+        <v>3005.5939999999991</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>7327</v>
+        <v>2235.9100000000017</v>
       </c>
       <c r="B50" s="0">
-        <v>3234</v>
+        <v>1762.1320000000005</v>
       </c>
       <c r="C50" s="0">
-        <v>3381</v>
+        <v>1902.9730000000004</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0">
-        <v>3887.4975000000031</v>
+        <v>16759.309999999994</v>
       </c>
       <c r="B51" s="0">
-        <v>2863.0859999999971</v>
+        <v>9248.1730000000025</v>
       </c>
       <c r="C51" s="0">
-        <v>3005.5939999999991</v>
+        <v>9299.146999999999</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0">
-        <v>5609</v>
+        <v>4869.9800000000023</v>
       </c>
       <c r="B52" s="0">
-        <v>5904</v>
+        <v>2704.0450000000005</v>
       </c>
       <c r="C52" s="0">
-        <v>5267</v>
+        <v>2941.7550000000001</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0">
-        <v>2235.9100000000017</v>
+        <v>5089.1450000000059</v>
       </c>
       <c r="B53" s="0">
-        <v>1762.1320000000005</v>
+        <v>2495.0159999999996</v>
       </c>
       <c r="C53" s="0">
-        <v>1902.9730000000004</v>
+        <v>2607.3530000000005</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0">
-        <v>4869.9800000000023</v>
+        <v>0</v>
       </c>
       <c r="B54" s="0">
-        <v>2704.0450000000005</v>
+        <v>0</v>
       </c>
       <c r="C54" s="0">
-        <v>2941.7550000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0">
-        <v>37817.099999999969</v>
+        <v>3381.9580000000005</v>
       </c>
       <c r="B55" s="0">
-        <v>14558.898999999996</v>
+        <v>2380.5339999999983</v>
       </c>
       <c r="C55" s="0">
-        <v>14776.000000000007</v>
+        <v>2428.5495000000019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0">
-        <v>5831</v>
+        <v>2284.5360000000001</v>
       </c>
       <c r="B56" s="0">
-        <v>2479</v>
+        <v>1891.0830000000001</v>
       </c>
       <c r="C56" s="0">
-        <v>2583</v>
+        <v>2068.4569999999999</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0">
-        <v>3381.9580000000005</v>
+        <v>12252.739999999998</v>
       </c>
       <c r="B57" s="0">
-        <v>2380.5339999999983</v>
+        <v>6782.1049999999932</v>
       </c>
       <c r="C57" s="0">
-        <v>2428.5495000000019</v>
+        <v>6758.3839999999964</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0">
-        <v>4039</v>
+        <v>4328.6750000000002</v>
       </c>
       <c r="B58" s="0">
-        <v>4239</v>
+        <v>2233.5149999999994</v>
       </c>
       <c r="C58" s="0">
-        <v>3796</v>
+        <v>2605.3999999999987</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0">
-        <v>2284.5360000000001</v>
+        <v>3628.4829999999993</v>
       </c>
       <c r="B59" s="0">
-        <v>1891.0830000000001</v>
+        <v>1841.2869999999996</v>
       </c>
       <c r="C59" s="0">
-        <v>2068.4569999999999</v>
+        <v>1956.3139999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0">
-        <v>4328.6750000000002</v>
+        <v>0</v>
       </c>
       <c r="B60" s="0">
-        <v>2233.5149999999994</v>
+        <v>0</v>
       </c>
       <c r="C60" s="0">
-        <v>2605.3999999999987</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">

</xml_diff>